<commit_message>
Added erf function prediction
</commit_message>
<xml_diff>
--- a/coronadata.xlsx
+++ b/coronadata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PC\Desktop\Corona\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D08C83E8-4908-4FC9-81D8-A8A30423C872}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC67AB29-21FA-4C2A-AC00-12FD1428C4B0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2AF399D8-4AE7-496D-BDBE-4F6A7218E433}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Suspeitos</t>
   </si>
@@ -48,6 +48,9 @@
   </si>
   <si>
     <t>Dia Ano</t>
+  </si>
+  <si>
+    <t>Confirmados_real</t>
   </si>
 </sst>
 </file>
@@ -399,20 +402,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD39D5D5-803D-4451-AF9A-F01477851509}">
-  <dimension ref="A1:E25"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G28" sqref="F28:G28"/>
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="9.140625" customWidth="1"/>
+    <col min="2" max="2" width="16.7109375" customWidth="1"/>
     <col min="3" max="4" width="15.140625" customWidth="1"/>
     <col min="5" max="5" width="13" customWidth="1"/>
+    <col min="6" max="6" width="17.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -428,8 +432,11 @@
       <c r="E1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>61</v>
       </c>
@@ -445,8 +452,12 @@
       <c r="E2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F2">
+        <f>C2-D2-E2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>62</v>
       </c>
@@ -462,8 +473,12 @@
       <c r="E3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F3">
+        <f t="shared" ref="F3:F25" si="0">C3-D3-E3</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>63</v>
       </c>
@@ -479,8 +494,12 @@
       <c r="E4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F4">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>64</v>
       </c>
@@ -496,8 +515,12 @@
       <c r="E5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F5">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>65</v>
       </c>
@@ -513,8 +536,12 @@
       <c r="E6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F6">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>66</v>
       </c>
@@ -530,8 +557,12 @@
       <c r="E7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F7">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>67</v>
       </c>
@@ -547,8 +578,12 @@
       <c r="E8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F8">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>68</v>
       </c>
@@ -564,8 +599,12 @@
       <c r="E9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F9">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>69</v>
       </c>
@@ -581,8 +620,12 @@
       <c r="E10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F10">
+        <f t="shared" si="0"/>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>70</v>
       </c>
@@ -598,8 +641,12 @@
       <c r="E11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F11">
+        <f t="shared" si="0"/>
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>71</v>
       </c>
@@ -615,8 +662,12 @@
       <c r="E12">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F12">
+        <f t="shared" si="0"/>
+        <v>59</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>72</v>
       </c>
@@ -632,8 +683,12 @@
       <c r="E13">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F13">
+        <f t="shared" si="0"/>
+        <v>77</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>73</v>
       </c>
@@ -649,8 +704,12 @@
       <c r="E14">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F14">
+        <f t="shared" si="0"/>
+        <v>111</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>74</v>
       </c>
@@ -666,8 +725,12 @@
       <c r="E15">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F15">
+        <f t="shared" si="0"/>
+        <v>167</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>75</v>
       </c>
@@ -683,8 +746,12 @@
       <c r="E16">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F16">
+        <f t="shared" si="0"/>
+        <v>243</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>76</v>
       </c>
@@ -700,8 +767,12 @@
       <c r="E17">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F17">
+        <f t="shared" si="0"/>
+        <v>328</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>77</v>
       </c>
@@ -717,8 +788,12 @@
       <c r="E18">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F18">
+        <f t="shared" si="0"/>
+        <v>444</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>78</v>
       </c>
@@ -734,8 +809,12 @@
       <c r="E19">
         <v>2</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F19">
+        <f t="shared" si="0"/>
+        <v>637</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>79</v>
       </c>
@@ -751,8 +830,12 @@
       <c r="E20">
         <v>3</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F20">
+        <f t="shared" si="0"/>
+        <v>779</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>80</v>
       </c>
@@ -768,8 +851,12 @@
       <c r="E21">
         <v>6</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F21">
+        <f t="shared" si="0"/>
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>81</v>
       </c>
@@ -785,8 +872,12 @@
       <c r="E22">
         <v>12</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F22">
+        <f t="shared" si="0"/>
+        <v>1263</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>82</v>
       </c>
@@ -802,8 +893,12 @@
       <c r="E23">
         <v>14</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F23">
+        <f t="shared" si="0"/>
+        <v>1581</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>83</v>
       </c>
@@ -819,8 +914,12 @@
       <c r="E24">
         <v>23</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F24">
+        <f t="shared" si="0"/>
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>84</v>
       </c>
@@ -835,6 +934,10 @@
       </c>
       <c r="E25">
         <v>30</v>
+      </c>
+      <c r="F25">
+        <f t="shared" si="0"/>
+        <v>2310</v>
       </c>
     </row>
   </sheetData>

</xml_diff>